<commit_message>
added optimal parameters algorithm
</commit_message>
<xml_diff>
--- a/efficiencies.xlsx
+++ b/efficiencies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javi/Documents/Padova/Research.nosync/ResearchActivities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99D1594-E30E-7541-8FEF-B833185494E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58407259-0DF6-D544-95FB-DF359468E19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33300" yWindow="1100" windowWidth="25440" windowHeight="14900" xr2:uid="{0698736A-FFBC-6246-9AAE-BD1A23F1A5CB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{0698736A-FFBC-6246-9AAE-BD1A23F1A5CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>HLT_Mu17_Photon30</t>
   </si>
@@ -135,6 +135,42 @@
   </si>
   <si>
     <t>38.75%</t>
+  </si>
+  <si>
+    <t>0.00002%</t>
+  </si>
+  <si>
+    <t>Muon1.pt &gt; 17.5,  Photon.pt &gt; 23.5, 2.25&lt;m(JPsi)&lt;3.5</t>
+  </si>
+  <si>
+    <t>25.13%</t>
+  </si>
+  <si>
+    <t>Muon1.pt &gt; 15.,  Photon.pt &gt; 23.5, 2.7&lt;m(JPsi)&lt;3.5</t>
+  </si>
+  <si>
+    <t>0.00005%</t>
+  </si>
+  <si>
+    <t>26.31%</t>
+  </si>
+  <si>
+    <t>37.68%</t>
+  </si>
+  <si>
+    <t>37.61%</t>
+  </si>
+  <si>
+    <t>Muon1.pt &gt; 20, Photon.pt &gt; 26.3, dR(mumu) &lt; 0.35</t>
+  </si>
+  <si>
+    <t>0.00008%</t>
+  </si>
+  <si>
+    <t>22.34%</t>
+  </si>
+  <si>
+    <t>36.62%</t>
   </si>
 </sst>
 </file>
@@ -695,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9626799-14FE-BA40-A51E-6B2121EA562C}">
-  <dimension ref="C4:N16"/>
+  <dimension ref="C4:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,17 +960,88 @@
         <v>32</v>
       </c>
     </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H24" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="I27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="H18:I18"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="G7:K9">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
added approx estimation of new efficiencies
</commit_message>
<xml_diff>
--- a/efficiencies.xlsx
+++ b/efficiencies.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javi/Documents/Padova/Research.nosync/ResearchActivities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C9CF50-CBEA-6249-8E30-9F230D5490DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79699CB1-DED6-5946-85D6-DBBE8FAFC328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1380" windowWidth="38400" windowHeight="21100" xr2:uid="{0698736A-FFBC-6246-9AAE-BD1A23F1A5CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>HLT_Mu17_Photon30</t>
   </si>
@@ -219,6 +219,15 @@
   </si>
   <si>
     <t>36.95</t>
+  </si>
+  <si>
+    <t>Muon1.pt &gt; 10, Muon2.pt &gt; 5, Photon.pt &gt; 22.7 2&lt;m(JPsi)&lt;4</t>
+  </si>
+  <si>
+    <t>28.21</t>
+  </si>
+  <si>
+    <t>38.90</t>
   </si>
 </sst>
 </file>
@@ -226,7 +235,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -546,10 +555,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -569,36 +578,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,31 +599,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -650,6 +623,45 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -967,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9626799-14FE-BA40-A51E-6B2121EA562C}">
-  <dimension ref="C4:O29"/>
+  <dimension ref="C4:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,59 +1000,61 @@
     <col min="13" max="13" width="39.5" style="1" customWidth="1"/>
     <col min="14" max="14" width="37.33203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="33.1640625" customWidth="1"/>
+    <col min="16" max="16" width="36" customWidth="1"/>
+    <col min="17" max="17" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="8"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="32"/>
     </row>
     <row r="5" spans="3:15" ht="17" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25" t="s">
+      <c r="I5" s="26"/>
+      <c r="J5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="30"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="18"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C6" s="4"/>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="17" t="s">
+      <c r="E6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -1061,19 +1075,19 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
-      <c r="O6" s="31"/>
+      <c r="O6" s="19"/>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1088,19 +1102,19 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="32"/>
+      <c r="O7" s="20"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1115,19 +1129,19 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="32"/>
+      <c r="O8" s="20"/>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="2" t="s">
         <v>33</v>
       </c>
@@ -1142,38 +1156,38 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="32"/>
+      <c r="O9" s="20"/>
     </row>
     <row r="10" spans="3:15" ht="17" x14ac:dyDescent="0.2">
       <c r="C10" s="3"/>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="21" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10" t="s">
+      <c r="G10" s="24"/>
+      <c r="H10" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="33"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="21"/>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C11" s="4"/>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="17"/>
+      <c r="E11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="10"/>
       <c r="G11" s="6" t="s">
         <v>7</v>
       </c>
@@ -1186,19 +1200,19 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="31"/>
+      <c r="O11" s="19"/>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="19"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1211,19 +1225,19 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="32"/>
+      <c r="O12" s="20"/>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="19"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1236,19 +1250,19 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="32"/>
+      <c r="O13" s="20"/>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="19"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1261,40 +1275,40 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="32"/>
+      <c r="O14" s="20"/>
     </row>
     <row r="15" spans="3:15" ht="17" x14ac:dyDescent="0.2">
       <c r="C15" s="3"/>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="21" t="s">
+      <c r="E15" s="28"/>
+      <c r="F15" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10" t="s">
+      <c r="G15" s="24"/>
+      <c r="H15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10" t="s">
+      <c r="I15" s="24"/>
+      <c r="J15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="34"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="22"/>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C16" s="4"/>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="17"/>
+      <c r="E16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="10"/>
       <c r="G16" s="6" t="s">
         <v>7</v>
       </c>
@@ -1309,19 +1323,19 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="31"/>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="O16" s="19"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1336,19 +1350,19 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="32"/>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="O17" s="20"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="19"/>
+      <c r="F18" s="12"/>
       <c r="G18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1363,19 +1377,19 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-      <c r="O18" s="32"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="O18" s="20"/>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="12"/>
       <c r="G19" s="2" t="s">
         <v>47</v>
       </c>
@@ -1390,44 +1404,48 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="32"/>
-    </row>
-    <row r="20" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="3:17" ht="17" x14ac:dyDescent="0.2">
       <c r="C20" s="4"/>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="21" t="s">
+      <c r="E20" s="28"/>
+      <c r="F20" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="9" t="s">
+      <c r="G20" s="27"/>
+      <c r="H20" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="26" t="s">
+      <c r="I20" s="24"/>
+      <c r="J20" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26" t="s">
+      <c r="K20" s="29"/>
+      <c r="L20" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26" t="s">
+      <c r="M20" s="29"/>
+      <c r="N20" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="29"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="O20" s="30"/>
+      <c r="P20" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q20" s="30"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C21" s="4"/>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="17"/>
+      <c r="E21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="10"/>
       <c r="G21" s="6" t="s">
         <v>7</v>
       </c>
@@ -1444,21 +1462,25 @@
         <v>7</v>
       </c>
       <c r="N21" s="2"/>
-      <c r="O21" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="O21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="19"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="2" t="s">
         <v>50</v>
       </c>
@@ -1475,21 +1497,25 @@
         <v>54</v>
       </c>
       <c r="N22" s="2"/>
-      <c r="O22" s="20" t="s">
+      <c r="O22" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="35"/>
+      <c r="Q22" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="2" t="s">
         <v>51</v>
       </c>
@@ -1506,21 +1532,25 @@
         <v>56</v>
       </c>
       <c r="N23" s="2"/>
-      <c r="O23" s="20" t="s">
+      <c r="O23" s="13" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="P23" s="35"/>
+      <c r="Q23" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="17"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="6" t="s">
         <v>52</v>
       </c>
@@ -1537,65 +1567,72 @@
         <v>59</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="20" t="s">
+      <c r="O24" s="13" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="3:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="D25" s="21" t="s">
+      <c r="P24" s="35"/>
+      <c r="Q24" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="D25" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="O25" s="28"/>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="D26" s="17" t="s">
+      <c r="E25" s="28"/>
+      <c r="O25" s="17"/>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="D26" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="O26" s="28"/>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="E26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O26" s="17"/>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="O27" s="28"/>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="G27" s="2"/>
+      <c r="O27" s="17"/>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="O28" s="28"/>
-    </row>
-    <row r="29" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
+      <c r="O28" s="17"/>
+    </row>
+    <row r="29" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="O29" s="28"/>
+      <c r="G29" s="6"/>
+      <c r="O29" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="D25:E25"/>
+  <mergeCells count="21">
+    <mergeCell ref="P20:Q20"/>
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="N20:O20"/>
@@ -1615,6 +1652,7 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D25:E25"/>
   </mergeCells>
   <conditionalFormatting sqref="G7:K9">
     <cfRule type="colorScale" priority="3">

</xml_diff>